<commit_message>
letzte Anpassung im Übungsszenariendokument
</commit_message>
<xml_diff>
--- a/01_Analyse/Analyse/04 Übungsszenarien/Uebungsszenarien_V1.0.xlsx
+++ b/01_Analyse/Analyse/04 Übungsszenarien/Uebungsszenarien_V1.0.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\quakrypto\01_Analyse\Analyse\04 Übungsszenarien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0757B55D-587F-4255-89CC-5458AF72A4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A0A8FA-692A-4270-907D-D4E59BC6EB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{536410C3-F7A2-4EA4-ABAC-DF979A666042}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{536410C3-F7A2-4EA4-ABAC-DF979A666042}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mitm" sheetId="6" r:id="rId1"/>
+    <sheet name="MITM" sheetId="6" r:id="rId1"/>
     <sheet name="Lauschangriff" sheetId="5" r:id="rId2"/>
     <sheet name="Normaler Ablauf" sheetId="7" r:id="rId3"/>
   </sheets>
@@ -2355,26 +2355,26 @@
   </sheetPr>
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="114" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
-    <col min="5" max="5" width="49.85546875" customWidth="1"/>
-    <col min="6" max="6" width="51.28515625" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="114" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.44140625" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" customWidth="1"/>
+    <col min="5" max="5" width="49.88671875" customWidth="1"/>
+    <col min="6" max="6" width="51.33203125" customWidth="1"/>
+    <col min="7" max="7" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" customWidth="1"/>
     <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="146.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="146.5546875" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="46" customFormat="1" ht="62.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="46" customFormat="1" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="111"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2389,7 +2389,7 @@
       <c r="J1" s="102"/>
       <c r="K1" s="111"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="111"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
@@ -2410,7 +2410,7 @@
       <c r="J2" s="102"/>
       <c r="K2" s="111"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="110"/>
       <c r="B4" s="60" t="s">
         <v>12</v>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="K4" s="110"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="110"/>
       <c r="B5" s="61" t="s">
         <v>17</v>
@@ -2496,7 +2496,7 @@
       </c>
       <c r="K5" s="110"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="110"/>
       <c r="B6" s="62" t="s">
         <v>20</v>
@@ -2520,7 +2520,7 @@
       </c>
       <c r="K6" s="110"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="110"/>
       <c r="B7" s="63" t="s">
         <v>23</v>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="K7" s="110"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="110"/>
       <c r="B8" s="64" t="s">
         <v>27</v>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="K8" s="110"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="110"/>
       <c r="B9" s="65" t="s">
         <v>31</v>
@@ -2606,7 +2606,7 @@
       </c>
       <c r="K9" s="110"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="110"/>
       <c r="B10" s="66" t="s">
         <v>33</v>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="K10" s="110"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="110"/>
       <c r="B11" s="67" t="s">
         <v>35</v>
@@ -2658,7 +2658,7 @@
       </c>
       <c r="K11" s="110"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="110"/>
       <c r="B12" s="68" t="s">
         <v>38</v>
@@ -2682,7 +2682,7 @@
       </c>
       <c r="K12" s="110"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>40</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>42</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="110"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2770,7 +2770,7 @@
       </c>
       <c r="K15" s="110"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="110"/>
       <c r="B16" s="1"/>
       <c r="C16" s="48" t="str">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="K16" s="110"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="110"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="K17" s="110"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="110"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="K18" s="110"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="110"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="K19" s="110"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="110"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="K20" s="110"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="110"/>
       <c r="B21" s="1"/>
       <c r="C21" s="70" t="str">
@@ -2936,7 +2936,7 @@
       </c>
       <c r="K21" s="110"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="110"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="K22" s="110"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="110"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2994,13 +2994,13 @@
       </c>
       <c r="K23" s="110"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="110"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="84" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="D24" s="84" t="str">
+        <f>F8</f>
+        <v>Int2 = 40</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>47</v>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="K24" s="110"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="110"/>
       <c r="B25" s="1"/>
       <c r="C25" s="70" t="str">
@@ -3055,7 +3055,7 @@
       </c>
       <c r="K25" s="110"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="110"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3080,7 +3080,7 @@
       </c>
       <c r="K26" s="110"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="110"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="K27" s="110"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="110"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="K28" s="110"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="110"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="K29" s="110"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="110"/>
       <c r="B30" s="1"/>
       <c r="C30" s="70" t="str">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="K30" s="110"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="110"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3218,7 +3218,7 @@
       </c>
       <c r="K31" s="110"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
         <v>94</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>96</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="110"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="K34" s="110"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="110"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3322,7 +3322,7 @@
       </c>
       <c r="K35" s="110"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="110"/>
       <c r="B36" s="1"/>
       <c r="C36" s="22" t="str">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="K36" s="110"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="110"/>
       <c r="B37" s="1"/>
       <c r="C37" s="21" t="str">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="K37" s="110"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="110"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="K38" s="110"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="110"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3436,7 +3436,7 @@
       </c>
       <c r="K39" s="110"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="110"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="K40" s="110"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="110"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="K41" s="110"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="110"/>
       <c r="B42" s="1"/>
       <c r="C42" s="70" t="str">
@@ -3517,7 +3517,7 @@
       </c>
       <c r="K42" s="110"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="110"/>
       <c r="B43" s="1"/>
       <c r="C43" s="42" t="str">
@@ -3549,7 +3549,7 @@
       </c>
       <c r="K43" s="110"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="110"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="K44" s="110"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="110"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3596,7 +3596,7 @@
       </c>
       <c r="K45" s="110"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="110"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3623,7 +3623,7 @@
       </c>
       <c r="K46" s="110"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="110"/>
       <c r="B47" s="1"/>
       <c r="C47" s="42" t="str">
@@ -3655,7 +3655,7 @@
       </c>
       <c r="K47" s="110"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="110"/>
       <c r="B48" s="1"/>
       <c r="C48" s="5"/>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="K48" s="110"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="110"/>
       <c r="B49" s="1"/>
       <c r="C49" s="5"/>
@@ -3704,7 +3704,7 @@
       </c>
       <c r="K49" s="110"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
         <v>123</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
         <v>127</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="110"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="K52" s="110"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="110"/>
       <c r="B53" s="1"/>
       <c r="C53" s="3" t="str">
@@ -3831,7 +3831,7 @@
       </c>
       <c r="K53" s="110"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="110"/>
       <c r="B54" s="1"/>
       <c r="C54" s="4" t="str">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="K54" s="110"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="110"/>
       <c r="B55" s="1"/>
       <c r="C55" s="4" t="str">
@@ -3895,7 +3895,7 @@
       </c>
       <c r="K55" s="110"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="110"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3920,7 +3920,7 @@
       </c>
       <c r="K56" s="110"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="110"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3942,7 +3942,7 @@
       </c>
       <c r="K57" s="110"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="110"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="K58" s="110"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="110"/>
       <c r="B59" s="1"/>
       <c r="C59" s="36" t="str">
@@ -4001,7 +4001,7 @@
       </c>
       <c r="K59" s="110"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="110"/>
       <c r="B60" s="1"/>
       <c r="C60" s="36" t="str">
@@ -4033,7 +4033,7 @@
       </c>
       <c r="K60" s="110"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="110"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -4058,7 +4058,7 @@
       </c>
       <c r="K61" s="110"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="110"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -4084,7 +4084,7 @@
       </c>
       <c r="K62" s="110"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="110"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="K63" s="110"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="110"/>
       <c r="B64" s="1"/>
       <c r="C64" s="35" t="str">
@@ -4145,7 +4145,7 @@
       </c>
       <c r="K64" s="110"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="110"/>
       <c r="B65" s="1"/>
       <c r="C65" s="36" t="str">
@@ -4177,7 +4177,7 @@
       </c>
       <c r="K65" s="110"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="110"/>
       <c r="B66" s="1"/>
       <c r="C66" s="36" t="str">
@@ -4209,7 +4209,7 @@
       </c>
       <c r="K66" s="110"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="110"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="K67" s="110"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="110"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4256,7 +4256,7 @@
       </c>
       <c r="K68" s="110"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="110"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4283,7 +4283,7 @@
       </c>
       <c r="K69" s="110"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="110"/>
       <c r="B70" s="1"/>
       <c r="C70" s="4" t="str">
@@ -4315,7 +4315,7 @@
       </c>
       <c r="K70" s="110"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="110"/>
       <c r="B71" s="1"/>
       <c r="C71" s="4" t="str">
@@ -4347,7 +4347,7 @@
       </c>
       <c r="K71" s="110"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="110"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="K72" s="110"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="110"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="K73" s="110"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="110"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4421,7 +4421,7 @@
       </c>
       <c r="K74" s="110"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="110"/>
       <c r="B75" s="1"/>
       <c r="C75" s="4" t="str">
@@ -4453,7 +4453,7 @@
       </c>
       <c r="K75" s="110"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="110"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4475,7 +4475,7 @@
       </c>
       <c r="K76" s="110"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="110"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4502,7 +4502,7 @@
       </c>
       <c r="K77" s="110"/>
     </row>
-    <row r="78" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="16" t="s">
         <v>183</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="17" t="s">
         <v>187</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="110"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4599,7 +4599,7 @@
       </c>
       <c r="K80" s="110"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="110"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -4621,7 +4621,7 @@
       </c>
       <c r="K81" s="110"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="110"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4648,7 +4648,7 @@
       </c>
       <c r="K82" s="110"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="110"/>
       <c r="B83" s="1"/>
       <c r="C83" s="29" t="str">
@@ -4681,7 +4681,7 @@
       </c>
       <c r="K83" s="110"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="110"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -4707,7 +4707,7 @@
       </c>
       <c r="K84" s="110"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="110"/>
       <c r="B85" s="1"/>
       <c r="C85" s="28" t="str">
@@ -4739,7 +4739,7 @@
       </c>
       <c r="K85" s="110"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="110"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -4763,7 +4763,7 @@
       </c>
       <c r="K86" s="110"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="110"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -4785,7 +4785,7 @@
       </c>
       <c r="K87" s="110"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="110"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -4812,7 +4812,7 @@
       </c>
       <c r="K88" s="110"/>
     </row>
-    <row r="89" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="16" t="s">
         <v>204</v>
       </c>
@@ -4870,22 +4870,22 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" customWidth="1"/>
-    <col min="5" max="5" width="50.85546875" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.140625" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="147.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" customWidth="1"/>
+    <col min="4" max="4" width="47.44140625" customWidth="1"/>
+    <col min="5" max="5" width="50.88671875" customWidth="1"/>
+    <col min="6" max="6" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.109375" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="147.5546875" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="62.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="111"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -4900,7 +4900,7 @@
       <c r="J1" s="102"/>
       <c r="K1" s="111"/>
     </row>
-    <row r="2" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="111"/>
       <c r="B2" s="123" t="s">
         <v>6</v>
@@ -4923,7 +4923,7 @@
       <c r="J2" s="102"/>
       <c r="K2" s="111"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="110"/>
       <c r="B4" s="115" t="s">
         <v>17</v>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="K4" s="110"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="110"/>
       <c r="B5" s="116" t="s">
         <v>20</v>
@@ -5009,7 +5009,7 @@
       </c>
       <c r="K5" s="110"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="110"/>
       <c r="B6" s="117" t="s">
         <v>23</v>
@@ -5033,7 +5033,7 @@
       </c>
       <c r="K6" s="110"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="110"/>
       <c r="B7" s="118" t="s">
         <v>27</v>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="K7" s="110"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="110"/>
       <c r="B8" s="119" t="s">
         <v>31</v>
@@ -5089,7 +5089,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="110"/>
       <c r="B9" s="120" t="s">
         <v>33</v>
@@ -5121,7 +5121,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="110"/>
       <c r="B10" s="121" t="s">
         <v>35</v>
@@ -5148,7 +5148,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>40</v>
       </c>
@@ -5179,7 +5179,7 @@
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>42</v>
       </c>
@@ -5215,7 +5215,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="110"/>
       <c r="C13" s="1"/>
       <c r="D13" s="84" t="str">
@@ -5246,7 +5246,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="110"/>
       <c r="C14" s="48" t="str">
         <f>F12</f>
@@ -5280,7 +5280,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="110"/>
       <c r="C15" s="1"/>
       <c r="D15" s="86" t="str">
@@ -5307,7 +5307,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="110"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -5331,7 +5331,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="129"/>
       <c r="C17" s="1"/>
@@ -5363,7 +5363,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="110"/>
       <c r="B18"/>
       <c r="C18" s="1"/>
@@ -5392,7 +5392,7 @@
       <c r="M18" s="44"/>
       <c r="N18" s="44"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="110"/>
       <c r="C19" s="70" t="str">
         <f>F17</f>
@@ -5426,7 +5426,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="110"/>
       <c r="C20" s="1"/>
       <c r="D20" s="130" t="str">
@@ -5457,7 +5457,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="110"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -5485,7 +5485,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="110"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -5510,7 +5510,7 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="110"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -5542,7 +5542,7 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="110"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -5571,7 +5571,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="110"/>
       <c r="B25" s="1"/>
       <c r="C25" s="70" t="str">
@@ -5606,7 +5606,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="110"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -5638,7 +5638,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>94</v>
       </c>
@@ -5667,7 +5667,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>96</v>
       </c>
@@ -5699,7 +5699,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="110"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -5724,7 +5724,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="110"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -5754,7 +5754,7 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="110"/>
       <c r="B31" s="1"/>
       <c r="C31" s="22" t="str">
@@ -5789,7 +5789,7 @@
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="110"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -5814,7 +5814,7 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="110"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -5844,7 +5844,7 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="110"/>
       <c r="B34" s="1"/>
       <c r="C34" s="70" t="str">
@@ -5879,7 +5879,7 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="110"/>
       <c r="B35" s="1"/>
       <c r="C35" s="42" t="str">
@@ -5914,7 +5914,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="110"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -5942,7 +5942,7 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="110"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -5967,7 +5967,7 @@
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="110"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -5997,7 +5997,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="110"/>
       <c r="B39" s="1"/>
       <c r="C39" s="42" t="str">
@@ -6032,7 +6032,7 @@
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="110"/>
       <c r="B40" s="1"/>
       <c r="C40" s="48" t="str">
@@ -6067,7 +6067,7 @@
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="110"/>
       <c r="B41" s="1"/>
       <c r="C41" s="5"/>
@@ -6092,7 +6092,7 @@
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="110"/>
       <c r="B42" s="1"/>
       <c r="C42" s="5"/>
@@ -6122,7 +6122,7 @@
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
     </row>
-    <row r="43" spans="1:14" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
         <v>123</v>
       </c>
@@ -6161,7 +6161,7 @@
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>127</v>
       </c>
@@ -6194,7 +6194,7 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="110"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -6226,7 +6226,7 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="110"/>
       <c r="B46" s="1"/>
       <c r="C46" s="3" t="str">
@@ -6261,7 +6261,7 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="110"/>
       <c r="B47" s="1"/>
       <c r="C47" s="4" t="str">
@@ -6296,7 +6296,7 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="110"/>
       <c r="B48" s="1"/>
       <c r="C48" s="4" t="str">
@@ -6331,7 +6331,7 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="110"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -6359,7 +6359,7 @@
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="110"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -6381,7 +6381,7 @@
       </c>
       <c r="K50" s="110"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="110"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -6408,7 +6408,7 @@
       </c>
       <c r="K51" s="110"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="110"/>
       <c r="B52" s="1"/>
       <c r="C52" s="36" t="str">
@@ -6440,7 +6440,7 @@
       </c>
       <c r="K52" s="110"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="110"/>
       <c r="B53" s="1"/>
       <c r="C53" s="36" t="str">
@@ -6472,7 +6472,7 @@
       </c>
       <c r="K53" s="110"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="110"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -6494,7 +6494,7 @@
       </c>
       <c r="K54" s="110"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="110"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -6521,7 +6521,7 @@
       </c>
       <c r="K55" s="110"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="110"/>
       <c r="B56" s="1"/>
       <c r="C56" s="4" t="str">
@@ -6553,7 +6553,7 @@
       </c>
       <c r="K56" s="110"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="110"/>
       <c r="B57" s="1"/>
       <c r="C57" s="4" t="str">
@@ -6585,7 +6585,7 @@
       </c>
       <c r="K57" s="110"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="110"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -6610,7 +6610,7 @@
       </c>
       <c r="K58" s="110"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="110"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -6632,7 +6632,7 @@
       </c>
       <c r="K59" s="110"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="110"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -6659,7 +6659,7 @@
       </c>
       <c r="K60" s="110"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="110"/>
       <c r="B61" s="1"/>
       <c r="C61" s="4" t="str">
@@ -6691,7 +6691,7 @@
       </c>
       <c r="K61" s="110"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="110"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -6713,7 +6713,7 @@
       </c>
       <c r="K62" s="110"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="110"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -6740,7 +6740,7 @@
       </c>
       <c r="K63" s="110"/>
     </row>
-    <row r="64" spans="1:14" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="16" t="s">
         <v>183</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
         <v>187</v>
       </c>
@@ -6812,7 +6812,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="110"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="K66" s="110"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="110"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -6859,7 +6859,7 @@
       </c>
       <c r="K67" s="110"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="110"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -6886,7 +6886,7 @@
       </c>
       <c r="K68" s="110"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="110"/>
       <c r="B69" s="1"/>
       <c r="C69" s="29" t="str">
@@ -6919,7 +6919,7 @@
       </c>
       <c r="K69" s="110"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="110"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="K70" s="110"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="110"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -6968,7 +6968,7 @@
       </c>
       <c r="K71" s="110"/>
     </row>
-    <row r="72" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="16" t="s">
         <v>204</v>
       </c>
@@ -7005,7 +7005,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="114"/>
     </row>
   </sheetData>
@@ -7029,21 +7029,21 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.140625" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="152.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="47.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.109375" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="152.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="62.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="61.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="111"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -7058,7 +7058,7 @@
       <c r="J1" s="102"/>
       <c r="K1" s="111"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="111"/>
       <c r="B2" s="123" t="s">
         <v>6</v>
@@ -7082,7 +7082,7 @@
       <c r="K2" s="111"/>
       <c r="L2" s="46"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
@@ -7113,7 +7113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="110"/>
       <c r="B4" s="115" t="s">
         <v>17</v>
@@ -7141,7 +7141,7 @@
       </c>
       <c r="K4" s="110"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="110"/>
       <c r="B5" s="116" t="s">
         <v>20</v>
@@ -7168,7 +7168,7 @@
       </c>
       <c r="K5" s="110"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="110"/>
       <c r="B6" s="117" t="s">
         <v>23</v>
@@ -7192,7 +7192,7 @@
       </c>
       <c r="K6" s="110"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="110"/>
       <c r="B7" s="118" t="s">
         <v>27</v>
@@ -7222,7 +7222,7 @@
       <c r="K7" s="110"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>40</v>
       </c>
@@ -7249,7 +7249,7 @@
       <c r="K8" s="111"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>42</v>
       </c>
@@ -7285,7 +7285,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="110"/>
       <c r="B10" s="121" t="s">
         <v>35</v>
@@ -7317,7 +7317,7 @@
       <c r="K10" s="110"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="110"/>
       <c r="B11" s="124" t="s">
         <v>38</v>
@@ -7352,7 +7352,7 @@
       <c r="K11" s="110"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="110"/>
       <c r="C12" s="1"/>
       <c r="D12" s="86" t="str">
@@ -7377,7 +7377,7 @@
       <c r="K12" s="110"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="110"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -7399,7 +7399,7 @@
       <c r="K13" s="110"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="110"/>
       <c r="C14" s="1"/>
       <c r="D14" s="84" t="str">
@@ -7428,7 +7428,7 @@
       <c r="K14" s="110"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="110"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -7455,7 +7455,7 @@
       <c r="K15" s="110"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="110"/>
       <c r="B16" s="1"/>
       <c r="C16" s="70" t="str">
@@ -7488,7 +7488,7 @@
       <c r="K16" s="110"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="110"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -7518,7 +7518,7 @@
       <c r="K17" s="110"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>94</v>
       </c>
@@ -7545,7 +7545,7 @@
       </c>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>96</v>
       </c>
@@ -7575,7 +7575,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="110"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -7598,7 +7598,7 @@
       <c r="K20" s="110"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="110"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -7626,7 +7626,7 @@
       <c r="K21" s="110"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="110"/>
       <c r="B22" s="1"/>
       <c r="C22" s="70" t="str">
@@ -7659,7 +7659,7 @@
       <c r="K22" s="110"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="110"/>
       <c r="B23" s="1"/>
       <c r="C23" s="42" t="str">
@@ -7692,7 +7692,7 @@
       <c r="K23" s="110"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="110"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -7718,7 +7718,7 @@
       <c r="K24" s="110"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="110"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -7741,7 +7741,7 @@
       <c r="K25" s="110"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="110"/>
       <c r="B26" s="1"/>
       <c r="C26" s="5"/>
@@ -7769,7 +7769,7 @@
       <c r="K26" s="110"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>123</v>
       </c>
@@ -7806,7 +7806,7 @@
       </c>
       <c r="L27" s="7"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>127</v>
       </c>
@@ -7840,7 +7840,7 @@
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="110"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -7870,7 +7870,7 @@
       <c r="K29" s="110"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="110"/>
       <c r="B30" s="1"/>
       <c r="C30" s="3" t="str">
@@ -7903,7 +7903,7 @@
       <c r="K30" s="110"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="110"/>
       <c r="B31" s="1"/>
       <c r="C31" s="4" t="str">
@@ -7936,7 +7936,7 @@
       <c r="K31" s="110"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="110"/>
       <c r="B32" s="1"/>
       <c r="C32" s="4" t="str">
@@ -7969,7 +7969,7 @@
       <c r="K32" s="110"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="110"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -7995,7 +7995,7 @@
       <c r="K33" s="110"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="110"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -8017,7 +8017,7 @@
       </c>
       <c r="K34" s="110"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="110"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -8044,7 +8044,7 @@
       </c>
       <c r="K35" s="110"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="110"/>
       <c r="B36" s="1"/>
       <c r="C36" s="4" t="str">
@@ -8076,7 +8076,7 @@
       </c>
       <c r="K36" s="110"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="110"/>
       <c r="B37" s="1"/>
       <c r="C37" s="4" t="str">
@@ -8108,7 +8108,7 @@
       </c>
       <c r="K37" s="110"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="110"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -8133,7 +8133,7 @@
       </c>
       <c r="K38" s="110"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="110"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -8155,7 +8155,7 @@
       </c>
       <c r="K39" s="110"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="110"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -8182,7 +8182,7 @@
       </c>
       <c r="K40" s="110"/>
     </row>
-    <row r="41" spans="1:12" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
         <v>183</v>
       </c>
@@ -8218,7 +8218,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>187</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="110"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -8279,7 +8279,7 @@
       </c>
       <c r="K43" s="110"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="110"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -8301,7 +8301,7 @@
       </c>
       <c r="K44" s="110"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="110"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -8328,7 +8328,7 @@
       </c>
       <c r="K45" s="110"/>
     </row>
-    <row r="46" spans="1:12" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" s="46" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
         <v>204</v>
       </c>
@@ -8365,7 +8365,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="114"/>
     </row>
   </sheetData>

</xml_diff>